<commit_message>
mise a jour de quelques doc du git
</commit_message>
<xml_diff>
--- a/paperasse/emploiDuTempsProjet.xlsx
+++ b/paperasse/emploiDuTempsProjet.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
   <si>
     <t>Créez un planning de projet dans cette feuille de calcul.
 Entrez le titre de ce projet dans la cellule B1. 
@@ -248,6 +248,9 @@
   </si>
   <si>
     <t>Developpement front-end du formulaire</t>
+  </si>
+  <si>
+    <t>programation des differentes trames du robot</t>
   </si>
 </sst>
 </file>
@@ -1281,6 +1284,30 @@
     <xf numFmtId="166" fontId="9" fillId="4" borderId="2" xfId="10" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="11" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -1299,30 +1326,6 @@
     </xf>
     <xf numFmtId="167" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="11" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1934,8 +1937,8 @@
   <dimension ref="A1:BL28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <pane ySplit="7" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1"/>
@@ -1989,131 +1992,131 @@
       <c r="B3" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="62" t="s">
+      <c r="C3" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="63"/>
-      <c r="E3" s="68">
+      <c r="D3" s="71"/>
+      <c r="E3" s="76">
         <v>44529</v>
       </c>
-      <c r="F3" s="68"/>
+      <c r="F3" s="76"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1">
       <c r="B4" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="63"/>
-      <c r="E4" s="68">
+      <c r="D4" s="71"/>
+      <c r="E4" s="76">
         <f>Début_Projet+11</f>
         <v>44540</v>
       </c>
-      <c r="F4" s="68"/>
+      <c r="F4" s="76"/>
     </row>
     <row r="5" spans="1:64" ht="30" customHeight="1">
       <c r="A5" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="62" t="s">
+      <c r="C5" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="63"/>
+      <c r="D5" s="71"/>
       <c r="E5" s="7">
         <v>1</v>
       </c>
-      <c r="I5" s="65">
+      <c r="I5" s="73">
         <f>I6</f>
         <v>44529</v>
       </c>
-      <c r="J5" s="66"/>
-      <c r="K5" s="66"/>
-      <c r="L5" s="66"/>
-      <c r="M5" s="66"/>
-      <c r="N5" s="66"/>
-      <c r="O5" s="67"/>
-      <c r="P5" s="65">
+      <c r="J5" s="74"/>
+      <c r="K5" s="74"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="74"/>
+      <c r="O5" s="75"/>
+      <c r="P5" s="73">
         <f>P6</f>
         <v>44536</v>
       </c>
-      <c r="Q5" s="66"/>
-      <c r="R5" s="66"/>
-      <c r="S5" s="66"/>
-      <c r="T5" s="66"/>
-      <c r="U5" s="66"/>
-      <c r="V5" s="67"/>
-      <c r="W5" s="65">
+      <c r="Q5" s="74"/>
+      <c r="R5" s="74"/>
+      <c r="S5" s="74"/>
+      <c r="T5" s="74"/>
+      <c r="U5" s="74"/>
+      <c r="V5" s="75"/>
+      <c r="W5" s="73">
         <f>W6</f>
         <v>44543</v>
       </c>
-      <c r="X5" s="66"/>
-      <c r="Y5" s="66"/>
-      <c r="Z5" s="66"/>
-      <c r="AA5" s="66"/>
-      <c r="AB5" s="66"/>
-      <c r="AC5" s="67"/>
-      <c r="AD5" s="65">
+      <c r="X5" s="74"/>
+      <c r="Y5" s="74"/>
+      <c r="Z5" s="74"/>
+      <c r="AA5" s="74"/>
+      <c r="AB5" s="74"/>
+      <c r="AC5" s="75"/>
+      <c r="AD5" s="73">
         <f>AD6</f>
         <v>44550</v>
       </c>
-      <c r="AE5" s="66"/>
-      <c r="AF5" s="66"/>
-      <c r="AG5" s="66"/>
-      <c r="AH5" s="66"/>
-      <c r="AI5" s="66"/>
-      <c r="AJ5" s="67"/>
-      <c r="AK5" s="65">
+      <c r="AE5" s="74"/>
+      <c r="AF5" s="74"/>
+      <c r="AG5" s="74"/>
+      <c r="AH5" s="74"/>
+      <c r="AI5" s="74"/>
+      <c r="AJ5" s="75"/>
+      <c r="AK5" s="73">
         <f>AK6</f>
         <v>44557</v>
       </c>
-      <c r="AL5" s="66"/>
-      <c r="AM5" s="66"/>
-      <c r="AN5" s="66"/>
-      <c r="AO5" s="66"/>
-      <c r="AP5" s="66"/>
-      <c r="AQ5" s="67"/>
-      <c r="AR5" s="65">
+      <c r="AL5" s="74"/>
+      <c r="AM5" s="74"/>
+      <c r="AN5" s="74"/>
+      <c r="AO5" s="74"/>
+      <c r="AP5" s="74"/>
+      <c r="AQ5" s="75"/>
+      <c r="AR5" s="73">
         <f>AR6</f>
         <v>44564</v>
       </c>
-      <c r="AS5" s="66"/>
-      <c r="AT5" s="66"/>
-      <c r="AU5" s="66"/>
-      <c r="AV5" s="66"/>
-      <c r="AW5" s="66"/>
-      <c r="AX5" s="67"/>
-      <c r="AY5" s="65">
+      <c r="AS5" s="74"/>
+      <c r="AT5" s="74"/>
+      <c r="AU5" s="74"/>
+      <c r="AV5" s="74"/>
+      <c r="AW5" s="74"/>
+      <c r="AX5" s="75"/>
+      <c r="AY5" s="73">
         <f>AY6</f>
         <v>44571</v>
       </c>
-      <c r="AZ5" s="66"/>
-      <c r="BA5" s="66"/>
-      <c r="BB5" s="66"/>
-      <c r="BC5" s="66"/>
-      <c r="BD5" s="66"/>
-      <c r="BE5" s="67"/>
-      <c r="BF5" s="65">
+      <c r="AZ5" s="74"/>
+      <c r="BA5" s="74"/>
+      <c r="BB5" s="74"/>
+      <c r="BC5" s="74"/>
+      <c r="BD5" s="74"/>
+      <c r="BE5" s="75"/>
+      <c r="BF5" s="73">
         <f>BF6</f>
         <v>44578</v>
       </c>
-      <c r="BG5" s="66"/>
-      <c r="BH5" s="66"/>
-      <c r="BI5" s="66"/>
-      <c r="BJ5" s="66"/>
-      <c r="BK5" s="66"/>
-      <c r="BL5" s="67"/>
+      <c r="BG5" s="74"/>
+      <c r="BH5" s="74"/>
+      <c r="BI5" s="74"/>
+      <c r="BJ5" s="74"/>
+      <c r="BK5" s="74"/>
+      <c r="BL5" s="75"/>
     </row>
     <row r="6" spans="1:64" ht="15" customHeight="1">
       <c r="A6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="64"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
       <c r="I6" s="57">
         <f>Début_Projet-WEEKDAY(Début_Projet,1)+2+7*(Semaine_Affichage-1)</f>
         <v>44529</v>
@@ -2158,7 +2161,7 @@
         <f t="shared" si="0"/>
         <v>44539</v>
       </c>
-      <c r="T6" s="74">
+      <c r="T6" s="67">
         <f t="shared" si="0"/>
         <v>44540</v>
       </c>
@@ -2402,15 +2405,15 @@
         <f t="shared" si="3"/>
         <v>m</v>
       </c>
-      <c r="S7" s="69" t="str">
+      <c r="S7" s="62" t="str">
         <f t="shared" si="3"/>
         <v>j</v>
       </c>
-      <c r="T7" s="75" t="str">
+      <c r="T7" s="68" t="str">
         <f t="shared" si="3"/>
         <v>v</v>
       </c>
-      <c r="U7" s="71" t="str">
+      <c r="U7" s="64" t="str">
         <f t="shared" si="3"/>
         <v>s</v>
       </c>
@@ -2607,9 +2610,9 @@
       <c r="P8" s="24"/>
       <c r="Q8" s="24"/>
       <c r="R8" s="24"/>
-      <c r="S8" s="70"/>
-      <c r="T8" s="76"/>
-      <c r="U8" s="72"/>
+      <c r="S8" s="63"/>
+      <c r="T8" s="69"/>
+      <c r="U8" s="65"/>
       <c r="V8" s="24"/>
       <c r="W8" s="24"/>
       <c r="X8" s="24"/>
@@ -2680,9 +2683,9 @@
       <c r="P9" s="24"/>
       <c r="Q9" s="24"/>
       <c r="R9" s="24"/>
-      <c r="S9" s="70"/>
-      <c r="T9" s="76"/>
-      <c r="U9" s="72"/>
+      <c r="S9" s="63"/>
+      <c r="T9" s="69"/>
+      <c r="U9" s="65"/>
       <c r="V9" s="24"/>
       <c r="W9" s="24"/>
       <c r="X9" s="24"/>
@@ -2763,9 +2766,9 @@
       <c r="P10" s="24"/>
       <c r="Q10" s="24"/>
       <c r="R10" s="24"/>
-      <c r="S10" s="70"/>
-      <c r="T10" s="76"/>
-      <c r="U10" s="72"/>
+      <c r="S10" s="63"/>
+      <c r="T10" s="69"/>
+      <c r="U10" s="65"/>
       <c r="V10" s="24"/>
       <c r="W10" s="24"/>
       <c r="X10" s="24"/>
@@ -2841,9 +2844,9 @@
       <c r="P11" s="24"/>
       <c r="Q11" s="24"/>
       <c r="R11" s="24"/>
-      <c r="S11" s="70"/>
-      <c r="T11" s="76"/>
-      <c r="U11" s="72"/>
+      <c r="S11" s="63"/>
+      <c r="T11" s="69"/>
+      <c r="U11" s="65"/>
       <c r="V11" s="24"/>
       <c r="W11" s="24"/>
       <c r="X11" s="24"/>
@@ -2924,9 +2927,9 @@
       <c r="P12" s="24"/>
       <c r="Q12" s="24"/>
       <c r="R12" s="24"/>
-      <c r="S12" s="70"/>
-      <c r="T12" s="76"/>
-      <c r="U12" s="73"/>
+      <c r="S12" s="63"/>
+      <c r="T12" s="69"/>
+      <c r="U12" s="66"/>
       <c r="V12" s="25"/>
       <c r="W12" s="24"/>
       <c r="X12" s="24"/>
@@ -3002,9 +3005,9 @@
       <c r="P13" s="24"/>
       <c r="Q13" s="24"/>
       <c r="R13" s="24"/>
-      <c r="S13" s="70"/>
-      <c r="T13" s="76"/>
-      <c r="U13" s="73"/>
+      <c r="S13" s="63"/>
+      <c r="T13" s="69"/>
+      <c r="U13" s="66"/>
       <c r="V13" s="25"/>
       <c r="W13" s="24"/>
       <c r="X13" s="24"/>
@@ -3080,9 +3083,9 @@
       <c r="P14" s="24"/>
       <c r="Q14" s="24"/>
       <c r="R14" s="24"/>
-      <c r="S14" s="70"/>
-      <c r="T14" s="76"/>
-      <c r="U14" s="73"/>
+      <c r="S14" s="63"/>
+      <c r="T14" s="69"/>
+      <c r="U14" s="66"/>
       <c r="V14" s="25"/>
       <c r="W14" s="24"/>
       <c r="X14" s="24"/>
@@ -3158,9 +3161,9 @@
       <c r="P15" s="24"/>
       <c r="Q15" s="24"/>
       <c r="R15" s="24"/>
-      <c r="S15" s="70"/>
-      <c r="T15" s="76"/>
-      <c r="U15" s="73"/>
+      <c r="S15" s="63"/>
+      <c r="T15" s="69"/>
+      <c r="U15" s="66"/>
       <c r="V15" s="25"/>
       <c r="W15" s="24"/>
       <c r="X15" s="24"/>
@@ -3229,9 +3232,9 @@
       <c r="P16" s="24"/>
       <c r="Q16" s="24"/>
       <c r="R16" s="24"/>
-      <c r="S16" s="70"/>
-      <c r="T16" s="76"/>
-      <c r="U16" s="72"/>
+      <c r="S16" s="63"/>
+      <c r="T16" s="69"/>
+      <c r="U16" s="65"/>
       <c r="V16" s="24"/>
       <c r="W16" s="24"/>
       <c r="X16" s="24"/>
@@ -3285,7 +3288,7 @@
         <v>50</v>
       </c>
       <c r="D17" s="19">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E17" s="61">
         <f>Début_Projet</f>
@@ -3310,9 +3313,9 @@
       <c r="P17" s="24"/>
       <c r="Q17" s="24"/>
       <c r="R17" s="24"/>
-      <c r="S17" s="70"/>
-      <c r="T17" s="76"/>
-      <c r="U17" s="72"/>
+      <c r="S17" s="63"/>
+      <c r="T17" s="69"/>
+      <c r="U17" s="65"/>
       <c r="V17" s="24"/>
       <c r="W17" s="24"/>
       <c r="X17" s="24"/>
@@ -3366,7 +3369,7 @@
         <v>44</v>
       </c>
       <c r="D18" s="19">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="E18" s="61">
         <f>Début_Projet+1</f>
@@ -3391,9 +3394,9 @@
       <c r="P18" s="24"/>
       <c r="Q18" s="24"/>
       <c r="R18" s="24"/>
-      <c r="S18" s="70"/>
-      <c r="T18" s="76"/>
-      <c r="U18" s="72"/>
+      <c r="S18" s="63"/>
+      <c r="T18" s="69"/>
+      <c r="U18" s="65"/>
       <c r="V18" s="24"/>
       <c r="W18" s="24"/>
       <c r="X18" s="24"/>
@@ -3474,9 +3477,9 @@
       <c r="P19" s="24"/>
       <c r="Q19" s="24"/>
       <c r="R19" s="24"/>
-      <c r="S19" s="70"/>
-      <c r="T19" s="76"/>
-      <c r="U19" s="72"/>
+      <c r="S19" s="63"/>
+      <c r="T19" s="69"/>
+      <c r="U19" s="65"/>
       <c r="V19" s="24"/>
       <c r="W19" s="24"/>
       <c r="X19" s="24"/>
@@ -3555,9 +3558,9 @@
       <c r="P20" s="24"/>
       <c r="Q20" s="24"/>
       <c r="R20" s="24"/>
-      <c r="S20" s="70"/>
-      <c r="T20" s="76"/>
-      <c r="U20" s="72"/>
+      <c r="S20" s="63"/>
+      <c r="T20" s="69"/>
+      <c r="U20" s="65"/>
       <c r="V20" s="24"/>
       <c r="W20" s="24"/>
       <c r="X20" s="24"/>
@@ -3604,16 +3607,22 @@
     </row>
     <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A21" s="38"/>
-      <c r="B21" s="50"/>
-      <c r="C21" s="48"/>
+      <c r="B21" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="48" t="s">
+        <v>44</v>
+      </c>
       <c r="D21" s="19">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="E21" s="61">
-        <v>44476</v>
+        <f>Début_Projet</f>
+        <v>44529</v>
       </c>
       <c r="F21" s="61">
-        <v>44484</v>
+        <f>E21+7</f>
+        <v>44536</v>
       </c>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
@@ -3627,9 +3636,9 @@
       <c r="P21" s="24"/>
       <c r="Q21" s="24"/>
       <c r="R21" s="24"/>
-      <c r="S21" s="70"/>
-      <c r="T21" s="76"/>
-      <c r="U21" s="72"/>
+      <c r="S21" s="63"/>
+      <c r="T21" s="69"/>
+      <c r="U21" s="65"/>
       <c r="V21" s="24"/>
       <c r="W21" s="24"/>
       <c r="X21" s="24"/>
@@ -3699,9 +3708,9 @@
       <c r="P22" s="24"/>
       <c r="Q22" s="24"/>
       <c r="R22" s="24"/>
-      <c r="S22" s="70"/>
-      <c r="T22" s="76"/>
-      <c r="U22" s="72"/>
+      <c r="S22" s="63"/>
+      <c r="T22" s="69"/>
+      <c r="U22" s="65"/>
       <c r="V22" s="24"/>
       <c r="W22" s="24"/>
       <c r="X22" s="24"/>
@@ -3771,9 +3780,9 @@
       <c r="P23" s="24"/>
       <c r="Q23" s="24"/>
       <c r="R23" s="24"/>
-      <c r="S23" s="70"/>
-      <c r="T23" s="76"/>
-      <c r="U23" s="72"/>
+      <c r="S23" s="63"/>
+      <c r="T23" s="69"/>
+      <c r="U23" s="65"/>
       <c r="V23" s="24"/>
       <c r="W23" s="24"/>
       <c r="X23" s="24"/>
@@ -3843,9 +3852,9 @@
       <c r="P24" s="24"/>
       <c r="Q24" s="24"/>
       <c r="R24" s="24"/>
-      <c r="S24" s="70"/>
-      <c r="T24" s="76"/>
-      <c r="U24" s="72"/>
+      <c r="S24" s="63"/>
+      <c r="T24" s="69"/>
+      <c r="U24" s="65"/>
       <c r="V24" s="24"/>
       <c r="W24" s="24"/>
       <c r="X24" s="24"/>
@@ -3914,9 +3923,9 @@
       <c r="P25" s="24"/>
       <c r="Q25" s="24"/>
       <c r="R25" s="24"/>
-      <c r="S25" s="70"/>
-      <c r="T25" s="76"/>
-      <c r="U25" s="72"/>
+      <c r="S25" s="63"/>
+      <c r="T25" s="69"/>
+      <c r="U25" s="65"/>
       <c r="V25" s="24"/>
       <c r="W25" s="24"/>
       <c r="X25" s="24"/>

</xml_diff>

<commit_message>
quelques docs en plus pour le passage a l'oral de lundi
</commit_message>
<xml_diff>
--- a/paperasse/emploiDuTempsProjet.xlsx
+++ b/paperasse/emploiDuTempsProjet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="2835" windowWidth="14400" windowHeight="7365"/>
@@ -19,7 +19,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">PlanningProjet!$5:$7</definedName>
     <definedName name="Semaine_Affichage">PlanningProjet!$E$5</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
   <si>
     <t>Créez un planning de projet dans cette feuille de calcul.
 Entrez le titre de ce projet dans la cellule B1. 
@@ -85,12 +85,6 @@
 Entrez la date de début de la tâche dans la cellule E9.
 Entrez la date de fin de tâche dans la cellule F9.
 Une barre d’état ombrée pour les dates entrées apparaît dans les blocs de la cellule I9 à la cellule BL9. </t>
-  </si>
-  <si>
-    <t>Les lignes 10 à 13 répètent le modèle de la ligne 9. 
-Répétez les instructions de la cellule A9 pour toutes les lignes de tâche dans cette feuille de calcul. Remplacez les exemples de données.
-Un exemple d’une autre phase commence à la cellule A14. 
-Continuez d’entrer des tâches dans les cellules A10 à A13, ou accédez à la cellule A14 pour en savoir plus.</t>
   </si>
   <si>
     <t>La cellule à droite contient l’exemple titre Phase 2. 
@@ -190,21 +184,9 @@
     <t>Gantt</t>
   </si>
   <si>
-    <t>Padey</t>
-  </si>
-  <si>
-    <t>Riviere</t>
-  </si>
-  <si>
     <t>Groupe</t>
   </si>
   <si>
-    <t>Auto apprentissage de nodeJS</t>
-  </si>
-  <si>
-    <t>Site node js</t>
-  </si>
-  <si>
     <t>Journal de bord</t>
   </si>
   <si>
@@ -229,12 +211,6 @@
     <t>Thomas</t>
   </si>
   <si>
-    <t>Creation et test de la class Araignée</t>
-  </si>
-  <si>
-    <t>Finalisation du formulaire</t>
-  </si>
-  <si>
     <t>Formation QT</t>
   </si>
   <si>
@@ -251,6 +227,12 @@
   </si>
   <si>
     <t>programation des differentes trames du robot</t>
+  </si>
+  <si>
+    <t>préparation des docs pour passage oral</t>
+  </si>
+  <si>
+    <t>Finalisation du formulaire (pauffinage)</t>
   </si>
 </sst>
 </file>
@@ -1308,6 +1290,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -1315,18 +1309,6 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="54">
     <cellStyle name="20 % - Accent1" xfId="31" builtinId="30" customBuiltin="1"/>
@@ -1633,7 +1615,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8638EF3-2DAE-40BC-A45A-2B8C536FAB0D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8638EF3-2DAE-40BC-A45A-2B8C536FAB0D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1642,10 +1624,10 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1923,7 +1905,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1934,11 +1916,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL28"/>
+  <dimension ref="A1:BL25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3:F3"/>
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1"/>
@@ -1963,7 +1945,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="42" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -1971,7 +1953,7 @@
       <c r="F1" s="26"/>
       <c r="H1" s="2"/>
       <c r="I1" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1">
@@ -1979,10 +1961,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I2" s="40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:64" ht="30" customHeight="1">
@@ -1990,133 +1972,133 @@
         <v>2</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" s="70" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="71"/>
-      <c r="E3" s="76">
+        <v>42</v>
+      </c>
+      <c r="C3" s="74" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="75"/>
+      <c r="E3" s="73">
         <v>44529</v>
       </c>
-      <c r="F3" s="76"/>
+      <c r="F3" s="73"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1">
       <c r="B4" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="70" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="71"/>
-      <c r="E4" s="76">
+        <v>43</v>
+      </c>
+      <c r="C4" s="74" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="75"/>
+      <c r="E4" s="73">
         <f>Début_Projet+11</f>
         <v>44540</v>
       </c>
-      <c r="F4" s="76"/>
+      <c r="F4" s="73"/>
     </row>
     <row r="5" spans="1:64" ht="30" customHeight="1">
       <c r="A5" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="70" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="71"/>
+      <c r="C5" s="74" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="75"/>
       <c r="E5" s="7">
         <v>1</v>
       </c>
-      <c r="I5" s="73">
+      <c r="I5" s="70">
         <f>I6</f>
         <v>44529</v>
       </c>
-      <c r="J5" s="74"/>
-      <c r="K5" s="74"/>
-      <c r="L5" s="74"/>
-      <c r="M5" s="74"/>
-      <c r="N5" s="74"/>
-      <c r="O5" s="75"/>
-      <c r="P5" s="73">
+      <c r="J5" s="71"/>
+      <c r="K5" s="71"/>
+      <c r="L5" s="71"/>
+      <c r="M5" s="71"/>
+      <c r="N5" s="71"/>
+      <c r="O5" s="72"/>
+      <c r="P5" s="70">
         <f>P6</f>
         <v>44536</v>
       </c>
-      <c r="Q5" s="74"/>
-      <c r="R5" s="74"/>
-      <c r="S5" s="74"/>
-      <c r="T5" s="74"/>
-      <c r="U5" s="74"/>
-      <c r="V5" s="75"/>
-      <c r="W5" s="73">
+      <c r="Q5" s="71"/>
+      <c r="R5" s="71"/>
+      <c r="S5" s="71"/>
+      <c r="T5" s="71"/>
+      <c r="U5" s="71"/>
+      <c r="V5" s="72"/>
+      <c r="W5" s="70">
         <f>W6</f>
         <v>44543</v>
       </c>
-      <c r="X5" s="74"/>
-      <c r="Y5" s="74"/>
-      <c r="Z5" s="74"/>
-      <c r="AA5" s="74"/>
-      <c r="AB5" s="74"/>
-      <c r="AC5" s="75"/>
-      <c r="AD5" s="73">
+      <c r="X5" s="71"/>
+      <c r="Y5" s="71"/>
+      <c r="Z5" s="71"/>
+      <c r="AA5" s="71"/>
+      <c r="AB5" s="71"/>
+      <c r="AC5" s="72"/>
+      <c r="AD5" s="70">
         <f>AD6</f>
         <v>44550</v>
       </c>
-      <c r="AE5" s="74"/>
-      <c r="AF5" s="74"/>
-      <c r="AG5" s="74"/>
-      <c r="AH5" s="74"/>
-      <c r="AI5" s="74"/>
-      <c r="AJ5" s="75"/>
-      <c r="AK5" s="73">
+      <c r="AE5" s="71"/>
+      <c r="AF5" s="71"/>
+      <c r="AG5" s="71"/>
+      <c r="AH5" s="71"/>
+      <c r="AI5" s="71"/>
+      <c r="AJ5" s="72"/>
+      <c r="AK5" s="70">
         <f>AK6</f>
         <v>44557</v>
       </c>
-      <c r="AL5" s="74"/>
-      <c r="AM5" s="74"/>
-      <c r="AN5" s="74"/>
-      <c r="AO5" s="74"/>
-      <c r="AP5" s="74"/>
-      <c r="AQ5" s="75"/>
-      <c r="AR5" s="73">
+      <c r="AL5" s="71"/>
+      <c r="AM5" s="71"/>
+      <c r="AN5" s="71"/>
+      <c r="AO5" s="71"/>
+      <c r="AP5" s="71"/>
+      <c r="AQ5" s="72"/>
+      <c r="AR5" s="70">
         <f>AR6</f>
         <v>44564</v>
       </c>
-      <c r="AS5" s="74"/>
-      <c r="AT5" s="74"/>
-      <c r="AU5" s="74"/>
-      <c r="AV5" s="74"/>
-      <c r="AW5" s="74"/>
-      <c r="AX5" s="75"/>
-      <c r="AY5" s="73">
+      <c r="AS5" s="71"/>
+      <c r="AT5" s="71"/>
+      <c r="AU5" s="71"/>
+      <c r="AV5" s="71"/>
+      <c r="AW5" s="71"/>
+      <c r="AX5" s="72"/>
+      <c r="AY5" s="70">
         <f>AY6</f>
         <v>44571</v>
       </c>
-      <c r="AZ5" s="74"/>
-      <c r="BA5" s="74"/>
-      <c r="BB5" s="74"/>
-      <c r="BC5" s="74"/>
-      <c r="BD5" s="74"/>
-      <c r="BE5" s="75"/>
-      <c r="BF5" s="73">
+      <c r="AZ5" s="71"/>
+      <c r="BA5" s="71"/>
+      <c r="BB5" s="71"/>
+      <c r="BC5" s="71"/>
+      <c r="BD5" s="71"/>
+      <c r="BE5" s="72"/>
+      <c r="BF5" s="70">
         <f>BF6</f>
         <v>44578</v>
       </c>
-      <c r="BG5" s="74"/>
-      <c r="BH5" s="74"/>
-      <c r="BI5" s="74"/>
-      <c r="BJ5" s="74"/>
-      <c r="BK5" s="74"/>
-      <c r="BL5" s="75"/>
+      <c r="BG5" s="71"/>
+      <c r="BH5" s="71"/>
+      <c r="BI5" s="71"/>
+      <c r="BJ5" s="71"/>
+      <c r="BK5" s="71"/>
+      <c r="BL5" s="72"/>
     </row>
     <row r="6" spans="1:64" ht="15" customHeight="1">
       <c r="A6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
+      <c r="B6" s="76"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="76"/>
       <c r="I6" s="57">
         <f>Début_Projet-WEEKDAY(Début_Projet,1)+2+7*(Semaine_Affichage-1)</f>
         <v>44529</v>
@@ -2347,23 +2329,23 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="E7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="F7" s="9" t="s">
         <v>17</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>18</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I7" s="10" t="str">
         <f t="shared" ref="I7:AN7" si="3">LEFT(TEXT(I6,"jjj"),1)</f>
@@ -2662,7 +2644,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="45"/>
       <c r="D9" s="15"/>
@@ -2670,7 +2652,7 @@
       <c r="F9" s="52"/>
       <c r="G9" s="13"/>
       <c r="H9" s="13" t="str">
-        <f t="shared" ref="H9:H25" si="5">IF(OR(ISBLANK(début_tâche),ISBLANK(fin_tâche)),"",fin_tâche-début_tâche+1)</f>
+        <f t="shared" ref="H9:H22" si="5">IF(OR(ISBLANK(début_tâche),ISBLANK(fin_tâche)),"",fin_tâche-début_tâche+1)</f>
         <v/>
       </c>
       <c r="I9" s="24"/>
@@ -2735,10 +2717,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="46" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D10" s="16">
         <v>1</v>
@@ -2816,10 +2798,10 @@
     <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A11" s="38"/>
       <c r="B11" s="49" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C11" s="46" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D11" s="16">
         <v>1</v>
@@ -2892,31 +2874,26 @@
       <c r="BL11" s="24"/>
     </row>
     <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A12" s="38" t="s">
-        <v>9</v>
-      </c>
+      <c r="A12" s="38"/>
       <c r="B12" s="49" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C12" s="46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D12" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" s="60">
-        <f>Début_Projet</f>
-        <v>44529</v>
+        <f>Début_Projet+4</f>
+        <v>44533</v>
       </c>
       <c r="F12" s="60">
-        <f>E12+4</f>
+        <f>E12</f>
         <v>44533</v>
       </c>
       <c r="G12" s="13"/>
-      <c r="H12" s="13">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
+      <c r="H12" s="13"/>
       <c r="I12" s="24"/>
       <c r="J12" s="24"/>
       <c r="K12" s="24"/>
@@ -2977,21 +2954,21 @@
     <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A13" s="38"/>
       <c r="B13" s="49" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C13" s="46" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D13" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="60">
-        <f>Début_Projet</f>
-        <v>44529</v>
+        <f>Début_Projet+11</f>
+        <v>44540</v>
       </c>
       <c r="F13" s="60">
-        <f>E13+3</f>
-        <v>44532</v>
+        <f>E13</f>
+        <v>44540</v>
       </c>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
@@ -3053,26 +3030,19 @@
       <c r="BL13" s="24"/>
     </row>
     <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A14" s="38"/>
-      <c r="B14" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="16">
-        <v>0</v>
-      </c>
-      <c r="E14" s="60">
-        <f>Début_Projet+4</f>
-        <v>44533</v>
-      </c>
-      <c r="F14" s="60">
-        <f>E14</f>
-        <v>44533</v>
-      </c>
+      <c r="A14" s="37"/>
+      <c r="B14" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="47"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="54"/>
       <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
+      <c r="H14" s="13" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="I14" s="24"/>
       <c r="J14" s="24"/>
       <c r="K14" s="24"/>
@@ -3085,8 +3055,8 @@
       <c r="R14" s="24"/>
       <c r="S14" s="63"/>
       <c r="T14" s="69"/>
-      <c r="U14" s="66"/>
-      <c r="V14" s="25"/>
+      <c r="U14" s="65"/>
+      <c r="V14" s="24"/>
       <c r="W14" s="24"/>
       <c r="X14" s="24"/>
       <c r="Y14" s="24"/>
@@ -3131,26 +3101,29 @@
       <c r="BL14" s="24"/>
     </row>
     <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A15" s="38"/>
-      <c r="B15" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="16">
-        <v>0</v>
-      </c>
-      <c r="E15" s="60">
-        <f>Début_Projet+11</f>
-        <v>44540</v>
-      </c>
-      <c r="F15" s="60">
-        <f>E15</f>
-        <v>44540</v>
+      <c r="A15" s="37"/>
+      <c r="B15" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="E15" s="61">
+        <f>Début_Projet</f>
+        <v>44529</v>
+      </c>
+      <c r="F15" s="61">
+        <f>E15+3</f>
+        <v>44532</v>
       </c>
       <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
+      <c r="H15" s="13">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
       <c r="I15" s="24"/>
       <c r="J15" s="24"/>
       <c r="K15" s="24"/>
@@ -3163,11 +3136,11 @@
       <c r="R15" s="24"/>
       <c r="S15" s="63"/>
       <c r="T15" s="69"/>
-      <c r="U15" s="66"/>
-      <c r="V15" s="25"/>
+      <c r="U15" s="65"/>
+      <c r="V15" s="24"/>
       <c r="W15" s="24"/>
       <c r="X15" s="24"/>
-      <c r="Y15" s="24"/>
+      <c r="Y15" s="25"/>
       <c r="Z15" s="24"/>
       <c r="AA15" s="24"/>
       <c r="AB15" s="24"/>
@@ -3209,18 +3182,30 @@
       <c r="BL15" s="24"/>
     </row>
     <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A16" s="37"/>
-      <c r="B16" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="47"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="54"/>
+      <c r="A16" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="19">
+        <v>0.33</v>
+      </c>
+      <c r="E16" s="61">
+        <f>F15</f>
+        <v>44532</v>
+      </c>
+      <c r="F16" s="61">
+        <f>E16+4</f>
+        <v>44536</v>
+      </c>
       <c r="G16" s="13"/>
-      <c r="H16" s="13" t="str">
+      <c r="H16" s="13">
         <f t="shared" si="5"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="I16" s="24"/>
       <c r="J16" s="24"/>
@@ -3280,23 +3265,23 @@
       <c r="BL16" s="24"/>
     </row>
     <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A17" s="37"/>
+      <c r="A17" s="38"/>
       <c r="B17" s="50" t="s">
         <v>53</v>
       </c>
       <c r="C17" s="48" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D17" s="19">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E17" s="61">
-        <f>Début_Projet</f>
-        <v>44529</v>
+        <f>F16</f>
+        <v>44536</v>
       </c>
       <c r="F17" s="61">
         <f>E17+3</f>
-        <v>44532</v>
+        <v>44539</v>
       </c>
       <c r="G17" s="13"/>
       <c r="H17" s="13">
@@ -3319,7 +3304,7 @@
       <c r="V17" s="24"/>
       <c r="W17" s="24"/>
       <c r="X17" s="24"/>
-      <c r="Y17" s="25"/>
+      <c r="Y17" s="24"/>
       <c r="Z17" s="24"/>
       <c r="AA17" s="24"/>
       <c r="AB17" s="24"/>
@@ -3361,29 +3346,26 @@
       <c r="BL17" s="24"/>
     </row>
     <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A18" s="37"/>
+      <c r="A18" s="38"/>
       <c r="B18" s="50" t="s">
         <v>51</v>
       </c>
       <c r="C18" s="48" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D18" s="19">
-        <v>0.15</v>
+        <v>0.4</v>
       </c>
       <c r="E18" s="61">
-        <f>Début_Projet+1</f>
-        <v>44530</v>
+        <f>Début_Projet</f>
+        <v>44529</v>
       </c>
       <c r="F18" s="61">
         <f>E18+7</f>
-        <v>44537</v>
+        <v>44536</v>
       </c>
       <c r="G18" s="13"/>
-      <c r="H18" s="13">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
+      <c r="H18" s="13"/>
       <c r="I18" s="24"/>
       <c r="J18" s="24"/>
       <c r="K18" s="24"/>
@@ -3442,31 +3424,26 @@
       <c r="BL18" s="24"/>
     </row>
     <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A19" s="38" t="s">
-        <v>10</v>
-      </c>
+      <c r="A19" s="38"/>
       <c r="B19" s="50" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C19" s="48" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D19" s="19">
         <v>0</v>
       </c>
       <c r="E19" s="61">
-        <f>F17</f>
-        <v>44532</v>
+        <f>E4-1</f>
+        <v>44539</v>
       </c>
       <c r="F19" s="61">
-        <f>E19+4</f>
-        <v>44536</v>
+        <f>E4</f>
+        <v>44540</v>
       </c>
       <c r="G19" s="13"/>
-      <c r="H19" s="13">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
+      <c r="H19" s="13"/>
       <c r="I19" s="24"/>
       <c r="J19" s="24"/>
       <c r="K19" s="24"/>
@@ -3526,28 +3503,19 @@
     </row>
     <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A20" s="38"/>
-      <c r="B20" s="50" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="48" t="s">
-        <v>54</v>
-      </c>
+      <c r="B20" s="50"/>
+      <c r="C20" s="48"/>
       <c r="D20" s="19">
         <v>0</v>
       </c>
       <c r="E20" s="61">
-        <f>F18</f>
-        <v>44537</v>
+        <v>44476</v>
       </c>
       <c r="F20" s="61">
-        <f>E20+3</f>
-        <v>44540</v>
+        <v>44484</v>
       </c>
       <c r="G20" s="13"/>
-      <c r="H20" s="13">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
+      <c r="H20" s="13"/>
       <c r="I20" s="24"/>
       <c r="J20" s="24"/>
       <c r="K20" s="24"/>
@@ -3607,22 +3575,16 @@
     </row>
     <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A21" s="38"/>
-      <c r="B21" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="48" t="s">
-        <v>44</v>
-      </c>
+      <c r="B21" s="50"/>
+      <c r="C21" s="48"/>
       <c r="D21" s="19">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="E21" s="61">
-        <f>Début_Projet</f>
-        <v>44529</v>
+        <v>44476</v>
       </c>
       <c r="F21" s="61">
-        <f>E21+7</f>
-        <v>44536</v>
+        <v>44484</v>
       </c>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
@@ -3684,20 +3646,19 @@
       <c r="BL21" s="24"/>
     </row>
     <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A22" s="38"/>
-      <c r="B22" s="50"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="19">
-        <v>0</v>
-      </c>
-      <c r="E22" s="61">
-        <v>44476</v>
-      </c>
-      <c r="F22" s="61">
-        <v>44484</v>
-      </c>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
+      <c r="A22" s="37"/>
+      <c r="B22" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="21"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="13" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="I22" s="24"/>
       <c r="J22" s="24"/>
       <c r="K22" s="24"/>
@@ -3755,233 +3716,25 @@
       <c r="BK22" s="24"/>
       <c r="BL22" s="24"/>
     </row>
-    <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A23" s="38"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="19">
-        <v>0</v>
-      </c>
-      <c r="E23" s="61">
-        <v>44476</v>
-      </c>
-      <c r="F23" s="61">
-        <v>44484</v>
-      </c>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="24"/>
-      <c r="K23" s="24"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="24"/>
-      <c r="N23" s="24"/>
-      <c r="O23" s="24"/>
-      <c r="P23" s="24"/>
-      <c r="Q23" s="24"/>
-      <c r="R23" s="24"/>
-      <c r="S23" s="63"/>
-      <c r="T23" s="69"/>
-      <c r="U23" s="65"/>
-      <c r="V23" s="24"/>
-      <c r="W23" s="24"/>
-      <c r="X23" s="24"/>
-      <c r="Y23" s="24"/>
-      <c r="Z23" s="24"/>
-      <c r="AA23" s="24"/>
-      <c r="AB23" s="24"/>
-      <c r="AC23" s="24"/>
-      <c r="AD23" s="24"/>
-      <c r="AE23" s="24"/>
-      <c r="AF23" s="24"/>
-      <c r="AG23" s="24"/>
-      <c r="AH23" s="24"/>
-      <c r="AI23" s="24"/>
-      <c r="AJ23" s="24"/>
-      <c r="AK23" s="24"/>
-      <c r="AL23" s="24"/>
-      <c r="AM23" s="24"/>
-      <c r="AN23" s="24"/>
-      <c r="AO23" s="24"/>
-      <c r="AP23" s="24"/>
-      <c r="AQ23" s="24"/>
-      <c r="AR23" s="24"/>
-      <c r="AS23" s="24"/>
-      <c r="AT23" s="24"/>
-      <c r="AU23" s="24"/>
-      <c r="AV23" s="24"/>
-      <c r="AW23" s="24"/>
-      <c r="AX23" s="24"/>
-      <c r="AY23" s="24"/>
-      <c r="AZ23" s="24"/>
-      <c r="BA23" s="24"/>
-      <c r="BB23" s="24"/>
-      <c r="BC23" s="24"/>
-      <c r="BD23" s="24"/>
-      <c r="BE23" s="24"/>
-      <c r="BF23" s="24"/>
-      <c r="BG23" s="24"/>
-      <c r="BH23" s="24"/>
-      <c r="BI23" s="24"/>
-      <c r="BJ23" s="24"/>
-      <c r="BK23" s="24"/>
-      <c r="BL23" s="24"/>
+    <row r="23" spans="1:64" ht="30" customHeight="1">
+      <c r="G23" s="6"/>
     </row>
-    <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A24" s="38"/>
-      <c r="B24" s="50"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="19">
-        <v>0</v>
-      </c>
-      <c r="E24" s="61">
-        <v>44476</v>
-      </c>
-      <c r="F24" s="61">
-        <v>44484</v>
-      </c>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="24"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="24"/>
-      <c r="N24" s="24"/>
-      <c r="O24" s="24"/>
-      <c r="P24" s="24"/>
-      <c r="Q24" s="24"/>
-      <c r="R24" s="24"/>
-      <c r="S24" s="63"/>
-      <c r="T24" s="69"/>
-      <c r="U24" s="65"/>
-      <c r="V24" s="24"/>
-      <c r="W24" s="24"/>
-      <c r="X24" s="24"/>
-      <c r="Y24" s="24"/>
-      <c r="Z24" s="24"/>
-      <c r="AA24" s="24"/>
-      <c r="AB24" s="24"/>
-      <c r="AC24" s="24"/>
-      <c r="AD24" s="24"/>
-      <c r="AE24" s="24"/>
-      <c r="AF24" s="24"/>
-      <c r="AG24" s="24"/>
-      <c r="AH24" s="24"/>
-      <c r="AI24" s="24"/>
-      <c r="AJ24" s="24"/>
-      <c r="AK24" s="24"/>
-      <c r="AL24" s="24"/>
-      <c r="AM24" s="24"/>
-      <c r="AN24" s="24"/>
-      <c r="AO24" s="24"/>
-      <c r="AP24" s="24"/>
-      <c r="AQ24" s="24"/>
-      <c r="AR24" s="24"/>
-      <c r="AS24" s="24"/>
-      <c r="AT24" s="24"/>
-      <c r="AU24" s="24"/>
-      <c r="AV24" s="24"/>
-      <c r="AW24" s="24"/>
-      <c r="AX24" s="24"/>
-      <c r="AY24" s="24"/>
-      <c r="AZ24" s="24"/>
-      <c r="BA24" s="24"/>
-      <c r="BB24" s="24"/>
-      <c r="BC24" s="24"/>
-      <c r="BD24" s="24"/>
-      <c r="BE24" s="24"/>
-      <c r="BF24" s="24"/>
-      <c r="BG24" s="24"/>
-      <c r="BH24" s="24"/>
-      <c r="BI24" s="24"/>
-      <c r="BJ24" s="24"/>
-      <c r="BK24" s="24"/>
-      <c r="BL24" s="24"/>
+    <row r="24" spans="1:64" ht="30" customHeight="1">
+      <c r="C24" s="11"/>
+      <c r="F24" s="39"/>
     </row>
-    <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A25" s="37"/>
-      <c r="B25" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" s="21"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="24"/>
-      <c r="N25" s="24"/>
-      <c r="O25" s="24"/>
-      <c r="P25" s="24"/>
-      <c r="Q25" s="24"/>
-      <c r="R25" s="24"/>
-      <c r="S25" s="63"/>
-      <c r="T25" s="69"/>
-      <c r="U25" s="65"/>
-      <c r="V25" s="24"/>
-      <c r="W25" s="24"/>
-      <c r="X25" s="24"/>
-      <c r="Y25" s="24"/>
-      <c r="Z25" s="24"/>
-      <c r="AA25" s="24"/>
-      <c r="AB25" s="24"/>
-      <c r="AC25" s="24"/>
-      <c r="AD25" s="24"/>
-      <c r="AE25" s="24"/>
-      <c r="AF25" s="24"/>
-      <c r="AG25" s="24"/>
-      <c r="AH25" s="24"/>
-      <c r="AI25" s="24"/>
-      <c r="AJ25" s="24"/>
-      <c r="AK25" s="24"/>
-      <c r="AL25" s="24"/>
-      <c r="AM25" s="24"/>
-      <c r="AN25" s="24"/>
-      <c r="AO25" s="24"/>
-      <c r="AP25" s="24"/>
-      <c r="AQ25" s="24"/>
-      <c r="AR25" s="24"/>
-      <c r="AS25" s="24"/>
-      <c r="AT25" s="24"/>
-      <c r="AU25" s="24"/>
-      <c r="AV25" s="24"/>
-      <c r="AW25" s="24"/>
-      <c r="AX25" s="24"/>
-      <c r="AY25" s="24"/>
-      <c r="AZ25" s="24"/>
-      <c r="BA25" s="24"/>
-      <c r="BB25" s="24"/>
-      <c r="BC25" s="24"/>
-      <c r="BD25" s="24"/>
-      <c r="BE25" s="24"/>
-      <c r="BF25" s="24"/>
-      <c r="BG25" s="24"/>
-      <c r="BH25" s="24"/>
-      <c r="BI25" s="24"/>
-      <c r="BJ25" s="24"/>
-      <c r="BK25" s="24"/>
-      <c r="BL25" s="24"/>
-    </row>
-    <row r="26" spans="1:64" ht="30" customHeight="1">
-      <c r="G26" s="6"/>
-    </row>
-    <row r="27" spans="1:64" ht="30" customHeight="1">
-      <c r="C27" s="11"/>
-      <c r="F27" s="39"/>
-    </row>
-    <row r="28" spans="1:64" ht="30" customHeight="1">
-      <c r="C28" s="12"/>
+    <row r="25" spans="1:64" ht="30" customHeight="1">
+      <c r="C25" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="AK5:AQ5"/>
+    <mergeCell ref="AR5:AX5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
     <mergeCell ref="AY5:BE5"/>
     <mergeCell ref="BF5:BL5"/>
     <mergeCell ref="E3:F3"/>
@@ -3989,15 +3742,8 @@
     <mergeCell ref="P5:V5"/>
     <mergeCell ref="W5:AC5"/>
     <mergeCell ref="AD5:AJ5"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="AK5:AQ5"/>
-    <mergeCell ref="AR5:AX5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D22:D25 D8:D20">
+  <conditionalFormatting sqref="D19:D22 D8:D17">
     <cfRule type="dataBar" priority="18">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4011,12 +3757,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I6:BL25">
+  <conditionalFormatting sqref="I6:BL22">
     <cfRule type="expression" dxfId="2" priority="37">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I8:BL25">
+  <conditionalFormatting sqref="I8:BL22">
     <cfRule type="expression" dxfId="1" priority="31">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -4024,7 +3770,7 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D21">
+  <conditionalFormatting sqref="D18">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4069,7 +3815,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D33</xm:sqref>
+          <xm:sqref>D7:D30</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4097,79 +3843,79 @@
     <row r="1" spans="1:2" ht="46.5" customHeight="1"/>
     <row r="2" spans="1:2" s="29" customFormat="1" ht="15.75">
       <c r="A2" s="28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="28"/>
     </row>
     <row r="3" spans="1:2" s="33" customFormat="1" ht="27" customHeight="1">
       <c r="A3" s="34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="34"/>
     </row>
     <row r="4" spans="1:2" s="30" customFormat="1" ht="26.25">
       <c r="A4" s="31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1">
       <c r="A5" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="26.25" customHeight="1">
       <c r="A6" s="31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="27" customFormat="1" ht="204.95" customHeight="1">
       <c r="A7" s="36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="30" customFormat="1" ht="26.25">
       <c r="A8" s="31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="81" customHeight="1">
       <c r="A9" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="27" customFormat="1" ht="27.95" customHeight="1">
       <c r="A10" s="35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="30" customFormat="1" ht="26.25">
       <c r="A11" s="31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="33.75" customHeight="1">
       <c r="A12" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="27" customFormat="1" ht="27.95" customHeight="1">
       <c r="A13" s="35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="30" customFormat="1" ht="26.25">
       <c r="A14" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="81.75" customHeight="1">
       <c r="A15" s="32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="90">
       <c r="A16" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
le code du robot et la paperasse mieu rempli
</commit_message>
<xml_diff>
--- a/paperasse/emploiDuTempsProjet.xlsx
+++ b/paperasse/emploiDuTempsProjet.xlsx
@@ -1920,7 +1920,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1"/>
@@ -2882,7 +2882,7 @@
         <v>37</v>
       </c>
       <c r="D12" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="60">
         <f>Début_Projet+4</f>
@@ -3109,7 +3109,7 @@
         <v>45</v>
       </c>
       <c r="D15" s="19">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E15" s="61">
         <f>Début_Projet</f>
@@ -3192,7 +3192,7 @@
         <v>45</v>
       </c>
       <c r="D16" s="19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="E16" s="61">
         <f>F15</f>
@@ -3354,7 +3354,7 @@
         <v>39</v>
       </c>
       <c r="D18" s="19">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="E18" s="61">
         <f>Début_Projet</f>
@@ -3432,7 +3432,7 @@
         <v>47</v>
       </c>
       <c r="D19" s="19">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="E19" s="61">
         <f>E4-1</f>

</xml_diff>